<commit_message>
Male promjene na gantu
</commit_message>
<xml_diff>
--- a/docs/gantt.xlsx
+++ b/docs/gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\Private\FER\Semestar8\Kolegiji\infsus\projekt\NeighbourConnect\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marko\Desktop\FAKS\DIPLOMSKI\2. SEMESTAR\INFSUS\PROJEKT\NeighbourConnect\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A028FD7-E5EE-4B40-BF5A-A938F60DB0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924C81D-BCDE-4C68-96CD-9A7D0473663C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D38409E-07F7-4C29-8230-484424FE2F6D}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{8D38409E-07F7-4C29-8230-484424FE2F6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>Početak razvoja frontend dijela sustava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Povezivanje frontend i backend dijela </t>
+  </si>
+  <si>
+    <t>Povezivanje baze podataka s aplikacijom</t>
+  </si>
+  <si>
+    <t>Deploy sustava (stavljen ovdje a ne pod implementaciju jer kao necemo pustat u pogon dok se ne testira sve)</t>
   </si>
 </sst>
 </file>
@@ -521,18 +530,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19335C74-4285-4BE1-906F-C12CEB6DEEAC}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,7 +562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -560,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -568,7 +578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -576,7 +586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -584,7 +594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -592,7 +602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -600,7 +610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -608,7 +618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -616,7 +626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -624,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -632,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -640,7 +650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -648,7 +658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -656,7 +666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -664,7 +674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -672,7 +682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -680,12 +690,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -693,7 +703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -701,7 +711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -709,7 +719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -717,7 +727,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -725,17 +735,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -743,7 +753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -751,7 +761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -759,7 +769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -767,42 +777,54 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grantic i jos nekaj
</commit_message>
<xml_diff>
--- a/docs/gantt.xlsx
+++ b/docs/gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marko\Desktop\FAKS\DIPLOMSKI\2. SEMESTAR\INFSUS\PROJEKT\NeighbourConnect\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marko\Desktop\FAKS\INFSUS\PROJEKT\NeighbourConnect\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924C81D-BCDE-4C68-96CD-9A7D0473663C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87C068D-65F1-41C3-80DD-D96188BEE618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{8D38409E-07F7-4C29-8230-484424FE2F6D}"/>
+    <workbookView xWindow="9312" yWindow="0" windowWidth="13824" windowHeight="12336" xr2:uid="{8D38409E-07F7-4C29-8230-484424FE2F6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -128,32 +128,165 @@
     <t>Izrada baze podataka</t>
   </si>
   <si>
-    <t>Početak razvoja backend dijela sustava</t>
-  </si>
-  <si>
-    <t>Početak razvoja frontend dijela sustava</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Povezivanje frontend i backend dijela </t>
-  </si>
-  <si>
     <t>Povezivanje baze podataka s aplikacijom</t>
   </si>
   <si>
-    <t>Deploy sustava (stavljen ovdje a ne pod implementaciju jer kao necemo pustat u pogon dok se ne testira sve)</t>
+    <t>Izrada jediničnih testova</t>
+  </si>
+  <si>
+    <t>Puštanje sustava u pogon</t>
+  </si>
+  <si>
+    <t>Povezivanje frontenda i backenda</t>
+  </si>
+  <si>
+    <t>Izrada integracijskih testova</t>
+  </si>
+  <si>
+    <t>Postavljanje testne razvojne okoline</t>
+  </si>
+  <si>
+    <t>Testiranje aplikacije u suradnji sa stanarima</t>
+  </si>
+  <si>
+    <t>06.03.2024</t>
+  </si>
+  <si>
+    <t>11.03.2024</t>
+  </si>
+  <si>
+    <t>12.03.2024</t>
+  </si>
+  <si>
+    <t>15.03.2024</t>
+  </si>
+  <si>
+    <t>13.03.2024</t>
+  </si>
+  <si>
+    <t>17.03.2024</t>
+  </si>
+  <si>
+    <t>30.03.2024</t>
+  </si>
+  <si>
+    <t>20.03.2024</t>
+  </si>
+  <si>
+    <t>2;3;4</t>
+  </si>
+  <si>
+    <t>18.03.2024</t>
+  </si>
+  <si>
+    <t>25.03.2024</t>
+  </si>
+  <si>
+    <t>31.03.2024</t>
+  </si>
+  <si>
+    <t>22.03.2024</t>
+  </si>
+  <si>
+    <t>23.03.2024</t>
+  </si>
+  <si>
+    <t>24.03.2024</t>
+  </si>
+  <si>
+    <t>26.03.2024</t>
+  </si>
+  <si>
+    <t>4;13</t>
+  </si>
+  <si>
+    <t>28.03.2024</t>
+  </si>
+  <si>
+    <t>14;15</t>
+  </si>
+  <si>
+    <t>05.04.2024</t>
+  </si>
+  <si>
+    <t>02.04.2024</t>
+  </si>
+  <si>
+    <t>04.04.2024</t>
+  </si>
+  <si>
+    <t>07.04.2024</t>
+  </si>
+  <si>
+    <t>08.04.2024</t>
+  </si>
+  <si>
+    <t>19;20</t>
+  </si>
+  <si>
+    <t>09.04.2024</t>
+  </si>
+  <si>
+    <t>15.04.2024</t>
+  </si>
+  <si>
+    <t>Razvoj backend dijela sustava</t>
+  </si>
+  <si>
+    <t>Razvoj frontend dijela sustava</t>
+  </si>
+  <si>
+    <t>01.05.2024</t>
+  </si>
+  <si>
+    <t>05.05.2024</t>
+  </si>
+  <si>
+    <t>20.04.2024</t>
+  </si>
+  <si>
+    <t>16.04.2024</t>
+  </si>
+  <si>
+    <t>22.05.2024</t>
+  </si>
+  <si>
+    <t>24.05.2024</t>
+  </si>
+  <si>
+    <t>26.05.2024</t>
+  </si>
+  <si>
+    <t>27;28;29;30</t>
+  </si>
+  <si>
+    <t>14.04.2024</t>
+  </si>
+  <si>
+    <t>08.05.2024</t>
+  </si>
+  <si>
+    <t>02.06.2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -192,13 +325,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -214,7 +348,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -530,19 +664,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19335C74-4285-4BE1-906F-C12CEB6DEEAC}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.90625" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -570,71 +706,158 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -642,60 +865,126 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -703,49 +992,88 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -753,63 +1081,126 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -817,18 +1208,72 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>